<commit_message>
good progress on the work flow in the R markdown document. i.e. set up dataset for functional diversity analysis and for the sensitivity analysis
</commit_message>
<xml_diff>
--- a/Functional traits all recorded species.xlsx
+++ b/Functional traits all recorded species.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grahamprescott/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grahamprescott/Rprojects/befta.birds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36127E4E-36B5-B149-B85A-92DB000A5DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BDB3F2-CA61-DE43-8AD4-F167B49D81B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1920" windowWidth="35380" windowHeight="20480" xr2:uid="{4C05C445-E994-2943-B906-1D820463732D}"/>
+    <workbookView xWindow="2840" yWindow="640" windowWidth="35380" windowHeight="20480" xr2:uid="{4C05C445-E994-2943-B906-1D820463732D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="177">
   <si>
     <t>SpecID</t>
   </si>
@@ -380,21 +380,6 @@
     <t>Christian</t>
   </si>
   <si>
-    <t>Strigiformes</t>
-  </si>
-  <si>
-    <t>Tytonidae</t>
-  </si>
-  <si>
-    <t>Barn owls</t>
-  </si>
-  <si>
-    <t>Tyto alba</t>
-  </si>
-  <si>
-    <t>Barn Owl</t>
-  </si>
-  <si>
     <t>Geopelia striata</t>
   </si>
   <si>
@@ -408,12 +393,6 @@
   </si>
   <si>
     <t>Woodpeckers</t>
-  </si>
-  <si>
-    <t>Dendrocopos moluccensis</t>
-  </si>
-  <si>
-    <t>Sunda Woodpecker</t>
   </si>
   <si>
     <t>Ref_7</t>
@@ -939,13 +918,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E09D457-BF0D-254E-859E-4213C7A53E03}">
-  <dimension ref="A1:AN29"/>
+  <dimension ref="A1:AN27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD1" sqref="AD1:AD1048576"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1114,34 +1093,34 @@
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>362</v>
+        <v>10860</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="F2">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>131</v>
+        <v>45</v>
       </c>
       <c r="J2">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1159,22 +1138,22 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="U2" t="s">
-        <v>132</v>
+        <v>47</v>
       </c>
       <c r="V2" t="s">
         <v>48</v>
@@ -1189,16 +1168,16 @@
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AB2">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AC2">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -1207,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="AF2" t="s">
-        <v>132</v>
+        <v>47</v>
       </c>
       <c r="AG2">
         <v>1</v>
@@ -1219,45 +1198,45 @@
         <v>0</v>
       </c>
       <c r="AJ2">
-        <v>751.72</v>
+        <v>8.1</v>
       </c>
       <c r="AK2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AL2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>934</v>
+        <v>10446</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="F3">
-        <v>95</v>
+        <v>159</v>
       </c>
       <c r="G3" t="s">
         <v>43</v>
       </c>
       <c r="H3" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
       <c r="J3">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1275,10 +1254,10 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -1290,7 +1269,7 @@
         <v>46</v>
       </c>
       <c r="U3" t="s">
-        <v>126</v>
+        <v>47</v>
       </c>
       <c r="V3" t="s">
         <v>48</v>
@@ -1305,16 +1284,16 @@
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AA3">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="AB3">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AD3">
         <v>0</v>
@@ -1323,7 +1302,7 @@
         <v>0</v>
       </c>
       <c r="AF3" t="s">
-        <v>126</v>
+        <v>47</v>
       </c>
       <c r="AG3">
         <v>1</v>
@@ -1335,42 +1314,42 @@
         <v>0</v>
       </c>
       <c r="AJ3">
-        <v>16.149999999999999</v>
+        <v>9.68</v>
       </c>
       <c r="AK3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AL3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1009</v>
+        <v>10074</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="F4">
-        <v>95</v>
+        <v>156</v>
       </c>
       <c r="G4" t="s">
         <v>43</v>
       </c>
       <c r="H4" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="I4" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="J4">
         <v>80</v>
@@ -1394,10 +1373,10 @@
         <v>10</v>
       </c>
       <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
         <v>10</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -1406,13 +1385,13 @@
         <v>46</v>
       </c>
       <c r="U4" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="V4" t="s">
         <v>48</v>
       </c>
       <c r="W4" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -1421,16 +1400,16 @@
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="AA4">
         <v>30</v>
       </c>
       <c r="AB4">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AC4">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AD4">
         <v>0</v>
@@ -1439,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="AF4" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="AG4">
         <v>1</v>
@@ -1451,7 +1430,7 @@
         <v>0</v>
       </c>
       <c r="AJ4">
-        <v>85.94</v>
+        <v>17.91</v>
       </c>
       <c r="AK4" t="s">
         <v>54</v>
@@ -1462,52 +1441,52 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1584</v>
+        <v>8271</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>128</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>129</v>
       </c>
       <c r="F5">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="G5" t="s">
         <v>43</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
       <c r="I5" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
       <c r="J5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -1519,34 +1498,34 @@
         <v>0</v>
       </c>
       <c r="T5" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="U5" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="V5" t="s">
         <v>48</v>
       </c>
       <c r="W5" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="X5">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
         <v>20</v>
       </c>
-      <c r="Z5">
-        <v>40</v>
-      </c>
       <c r="AA5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AC5">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AD5">
         <v>0</v>
@@ -1555,19 +1534,19 @@
         <v>0</v>
       </c>
       <c r="AF5" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="AG5">
         <v>1</v>
       </c>
       <c r="AH5" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="AI5">
         <v>0</v>
       </c>
       <c r="AJ5">
-        <v>91.4</v>
+        <v>82.6</v>
       </c>
       <c r="AK5" t="s">
         <v>54</v>
@@ -1578,43 +1557,43 @@
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1759</v>
+        <v>4669</v>
       </c>
       <c r="B6" t="s">
         <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>167</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
       <c r="F6">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
         <v>43</v>
       </c>
       <c r="H6" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="I6" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="J6">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1623,7 +1602,7 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -1635,16 +1614,16 @@
         <v>0</v>
       </c>
       <c r="T6" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="U6" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="V6" t="s">
         <v>48</v>
       </c>
       <c r="W6" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -1653,16 +1632,16 @@
         <v>0</v>
       </c>
       <c r="Z6">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AA6">
         <v>0</v>
       </c>
       <c r="AB6">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="AC6">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -1671,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="AF6" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="AG6">
         <v>1</v>
@@ -1683,7 +1662,7 @@
         <v>0</v>
       </c>
       <c r="AJ6">
-        <v>25.3</v>
+        <v>597.74</v>
       </c>
       <c r="AK6" t="s">
         <v>54</v>
@@ -1694,37 +1673,37 @@
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1834</v>
+        <v>2377</v>
       </c>
       <c r="B7" t="s">
         <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>174</v>
       </c>
       <c r="F7">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="G7" t="s">
         <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>88</v>
+        <v>175</v>
       </c>
       <c r="I7" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="J7">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="K7">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1739,28 +1718,28 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="S7">
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="U7" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="V7" t="s">
         <v>48</v>
       </c>
       <c r="W7" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="X7">
         <v>0</v>
@@ -1769,10 +1748,10 @@
         <v>0</v>
       </c>
       <c r="Z7">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="AA7">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AB7">
         <v>0</v>
@@ -1781,25 +1760,25 @@
         <v>0</v>
       </c>
       <c r="AD7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AE7">
         <v>0</v>
       </c>
       <c r="AF7" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="AG7">
         <v>1</v>
       </c>
       <c r="AH7" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="AI7">
         <v>0</v>
       </c>
       <c r="AJ7">
-        <v>280.7</v>
+        <v>10.7</v>
       </c>
       <c r="AK7" t="s">
         <v>54</v>
@@ -1810,34 +1789,34 @@
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2377</v>
+        <v>11778</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>179</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="E8" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="F8">
-        <v>77</v>
+        <v>183</v>
       </c>
       <c r="G8" t="s">
         <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>182</v>
+        <v>145</v>
       </c>
       <c r="I8" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
       <c r="J8">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1861,22 +1840,22 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="U8" t="s">
-        <v>112</v>
+        <v>147</v>
       </c>
       <c r="V8" t="s">
         <v>48</v>
       </c>
       <c r="W8" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -1885,37 +1864,37 @@
         <v>0</v>
       </c>
       <c r="Z8">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AA8">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AB8">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AC8">
         <v>0</v>
       </c>
       <c r="AD8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AE8">
         <v>0</v>
       </c>
       <c r="AF8" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="AG8">
         <v>1</v>
       </c>
       <c r="AH8" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="AI8">
         <v>0</v>
       </c>
       <c r="AJ8">
-        <v>10.7</v>
+        <v>21.39</v>
       </c>
       <c r="AK8" t="s">
         <v>54</v>
@@ -1926,73 +1905,73 @@
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2878</v>
+        <v>9922</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="F9">
-        <v>70</v>
+        <v>154</v>
       </c>
       <c r="G9" t="s">
         <v>43</v>
       </c>
       <c r="H9" t="s">
-        <v>117</v>
+        <v>74</v>
       </c>
       <c r="I9" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="J9">
+        <v>40</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
         <v>10</v>
       </c>
-      <c r="K9">
-        <v>80</v>
-      </c>
-      <c r="L9">
+      <c r="P9">
+        <v>20</v>
+      </c>
+      <c r="Q9">
         <v>10</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
       <c r="R9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="U9" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="V9" t="s">
         <v>48</v>
       </c>
       <c r="W9" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="X9">
         <v>0</v>
@@ -2001,16 +1980,16 @@
         <v>0</v>
       </c>
       <c r="Z9">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="AA9">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AB9">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AC9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AD9">
         <v>0</v>
@@ -2019,19 +1998,19 @@
         <v>0</v>
       </c>
       <c r="AF9" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="AG9">
         <v>1</v>
       </c>
       <c r="AH9" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="AI9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ9">
-        <v>403.32</v>
+        <v>16.25</v>
       </c>
       <c r="AK9" t="s">
         <v>54</v>
@@ -2042,37 +2021,37 @@
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>3171</v>
+        <v>1834</v>
       </c>
       <c r="B10" t="s">
         <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="E10" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="F10">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G10" t="s">
         <v>43</v>
       </c>
       <c r="H10" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="I10" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="J10">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -2087,28 +2066,28 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S10">
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="U10" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="V10" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="W10" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="X10">
         <v>0</v>
@@ -2117,13 +2096,13 @@
         <v>0</v>
       </c>
       <c r="Z10">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="AA10">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="AB10">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AC10">
         <v>0</v>
@@ -2135,57 +2114,57 @@
         <v>0</v>
       </c>
       <c r="AF10" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="AG10">
         <v>1</v>
       </c>
       <c r="AH10" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="AI10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ10">
-        <v>85.86</v>
+        <v>280.7</v>
       </c>
       <c r="AK10" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AL10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>3385</v>
+        <v>10220</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F11">
-        <v>65</v>
+        <v>160</v>
       </c>
       <c r="G11" t="s">
         <v>43</v>
       </c>
       <c r="H11" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="I11" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -2203,22 +2182,22 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="S11">
         <v>0</v>
       </c>
       <c r="T11" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="U11" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="V11" t="s">
         <v>48</v>
@@ -2233,13 +2212,13 @@
         <v>0</v>
       </c>
       <c r="Z11">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AB11">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="AC11">
         <v>0</v>
@@ -2251,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="AF11" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="AG11">
         <v>1</v>
@@ -2263,7 +2242,7 @@
         <v>0</v>
       </c>
       <c r="AJ11">
-        <v>159</v>
+        <v>34.85</v>
       </c>
       <c r="AK11" t="s">
         <v>54</v>
@@ -2274,34 +2253,34 @@
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>3433</v>
+        <v>9277</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="F12">
-        <v>65</v>
+        <v>167</v>
       </c>
       <c r="G12" t="s">
         <v>43</v>
       </c>
       <c r="H12" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="I12" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="J12">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -2313,34 +2292,34 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R12">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="S12">
         <v>0</v>
       </c>
       <c r="T12" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="U12" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="V12" t="s">
         <v>48</v>
       </c>
       <c r="W12" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="X12">
         <v>0</v>
@@ -2349,10 +2328,10 @@
         <v>0</v>
       </c>
       <c r="Z12">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="AA12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB12">
         <v>0</v>
@@ -2367,7 +2346,7 @@
         <v>0</v>
       </c>
       <c r="AF12" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="AG12">
         <v>1</v>
@@ -2379,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="AJ12">
-        <v>56.6</v>
+        <v>36</v>
       </c>
       <c r="AK12" t="s">
         <v>54</v>
@@ -2390,34 +2369,34 @@
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>3880</v>
+        <v>8395</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>157</v>
+        <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>158</v>
+        <v>100</v>
       </c>
       <c r="F13">
-        <v>42</v>
+        <v>145</v>
       </c>
       <c r="G13" t="s">
         <v>43</v>
       </c>
       <c r="H13" t="s">
-        <v>159</v>
+        <v>101</v>
       </c>
       <c r="I13" t="s">
-        <v>160</v>
+        <v>102</v>
       </c>
       <c r="J13">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -2426,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -2441,37 +2420,37 @@
         <v>0</v>
       </c>
       <c r="R13">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="S13">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T13" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="U13" t="s">
-        <v>161</v>
+        <v>47</v>
       </c>
       <c r="V13" t="s">
         <v>48</v>
       </c>
       <c r="W13" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="X13">
         <v>0</v>
       </c>
       <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
         <v>20</v>
-      </c>
-      <c r="Z13">
-        <v>60</v>
       </c>
       <c r="AA13">
         <v>20</v>
       </c>
       <c r="AB13">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AC13">
         <v>0</v>
@@ -2483,19 +2462,19 @@
         <v>0</v>
       </c>
       <c r="AF13" t="s">
-        <v>161</v>
+        <v>47</v>
       </c>
       <c r="AG13">
         <v>1</v>
       </c>
       <c r="AH13" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="AI13">
         <v>0</v>
       </c>
       <c r="AJ13">
-        <v>180</v>
+        <v>12.5</v>
       </c>
       <c r="AK13" t="s">
         <v>54</v>
@@ -2506,53 +2485,53 @@
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>4669</v>
+        <v>11221</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>174</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
       <c r="E14" t="s">
-        <v>176</v>
+        <v>140</v>
       </c>
       <c r="F14">
-        <v>36</v>
+        <v>163</v>
       </c>
       <c r="G14" t="s">
         <v>43</v>
       </c>
       <c r="H14" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
       <c r="I14" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
       <c r="J14">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
         <v>20</v>
       </c>
-      <c r="L14">
-        <v>60</v>
-      </c>
-      <c r="M14">
-        <v>10</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
       <c r="Q14">
         <v>0</v>
       </c>
@@ -2563,10 +2542,10 @@
         <v>0</v>
       </c>
       <c r="T14" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="U14" t="s">
-        <v>132</v>
+        <v>76</v>
       </c>
       <c r="V14" t="s">
         <v>48</v>
@@ -2581,16 +2560,16 @@
         <v>0</v>
       </c>
       <c r="Z14">
+        <v>20</v>
+      </c>
+      <c r="AA14">
         <v>50</v>
       </c>
-      <c r="AA14">
-        <v>0</v>
-      </c>
       <c r="AB14">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="AC14">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -2599,7 +2578,7 @@
         <v>0</v>
       </c>
       <c r="AF14" t="s">
-        <v>132</v>
+        <v>47</v>
       </c>
       <c r="AG14">
         <v>1</v>
@@ -2611,7 +2590,7 @@
         <v>0</v>
       </c>
       <c r="AJ14">
-        <v>597.74</v>
+        <v>11.83</v>
       </c>
       <c r="AK14" t="s">
         <v>54</v>
@@ -2622,40 +2601,40 @@
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>8079</v>
+        <v>1759</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>169</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
-        <v>170</v>
+        <v>87</v>
       </c>
       <c r="F15">
-        <v>147</v>
+        <v>67</v>
       </c>
       <c r="G15" t="s">
         <v>43</v>
       </c>
       <c r="H15" t="s">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="I15" t="s">
-        <v>172</v>
+        <v>127</v>
       </c>
       <c r="J15">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -2664,10 +2643,10 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -2679,10 +2658,10 @@
         <v>0</v>
       </c>
       <c r="T15" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="U15" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
       <c r="V15" t="s">
         <v>48</v>
@@ -2697,37 +2676,37 @@
         <v>0</v>
       </c>
       <c r="Z15">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AA15">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AB15">
+        <v>40</v>
+      </c>
+      <c r="AC15">
+        <v>60</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG15">
+        <v>1</v>
+      </c>
+      <c r="AH15" t="s">
         <v>50</v>
       </c>
-      <c r="AC15">
-        <v>0</v>
-      </c>
-      <c r="AD15">
-        <v>0</v>
-      </c>
-      <c r="AE15">
-        <v>0</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>173</v>
-      </c>
-      <c r="AG15">
-        <v>1</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>113</v>
-      </c>
       <c r="AI15">
         <v>0</v>
       </c>
       <c r="AJ15">
-        <v>251</v>
+        <v>25.3</v>
       </c>
       <c r="AK15" t="s">
         <v>54</v>
@@ -2738,34 +2717,34 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>8230</v>
+        <v>362</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="E16" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
       <c r="F16">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="G16" t="s">
         <v>43</v>
       </c>
       <c r="H16" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="I16" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="J16">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -2783,28 +2762,28 @@
         <v>0</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q16">
         <v>0</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T16" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="U16" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="V16" t="s">
         <v>48</v>
       </c>
       <c r="W16" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="X16">
         <v>0</v>
@@ -2813,7 +2792,7 @@
         <v>0</v>
       </c>
       <c r="Z16">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AA16">
         <v>0</v>
@@ -2825,13 +2804,13 @@
         <v>0</v>
       </c>
       <c r="AD16">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AE16">
         <v>0</v>
       </c>
       <c r="AF16" t="s">
-        <v>166</v>
+        <v>125</v>
       </c>
       <c r="AG16">
         <v>1</v>
@@ -2843,7 +2822,7 @@
         <v>0</v>
       </c>
       <c r="AJ16">
-        <v>41.69</v>
+        <v>751.72</v>
       </c>
       <c r="AK16" t="s">
         <v>54</v>
@@ -2854,56 +2833,56 @@
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>8271</v>
+        <v>1009</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="F17">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="G17" t="s">
         <v>43</v>
       </c>
       <c r="H17" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="I17" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="J17">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
         <v>10</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
+      <c r="Q17">
         <v>10</v>
       </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>60</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
       <c r="R17">
         <v>0</v>
       </c>
@@ -2911,16 +2890,16 @@
         <v>0</v>
       </c>
       <c r="T17" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="U17" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="V17" t="s">
         <v>48</v>
       </c>
       <c r="W17" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="X17">
         <v>0</v>
@@ -2929,16 +2908,16 @@
         <v>0</v>
       </c>
       <c r="Z17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AA17">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="AB17">
         <v>30</v>
       </c>
       <c r="AC17">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="AD17">
         <v>0</v>
@@ -2947,19 +2926,19 @@
         <v>0</v>
       </c>
       <c r="AF17" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="AG17">
         <v>1</v>
       </c>
       <c r="AH17" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="AI17">
         <v>0</v>
       </c>
       <c r="AJ17">
-        <v>82.6</v>
+        <v>85.94</v>
       </c>
       <c r="AK17" t="s">
         <v>54</v>
@@ -2970,7 +2949,7 @@
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>8395</v>
+        <v>10859</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
@@ -2979,22 +2958,22 @@
         <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="F18">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="G18" t="s">
         <v>43</v>
       </c>
       <c r="H18" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="I18" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="J18">
         <v>100</v>
@@ -3045,13 +3024,13 @@
         <v>0</v>
       </c>
       <c r="Z18">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA18">
         <v>20</v>
       </c>
       <c r="AB18">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="AC18">
         <v>0</v>
@@ -3075,7 +3054,7 @@
         <v>0</v>
       </c>
       <c r="AJ18">
-        <v>12.5</v>
+        <v>10.8</v>
       </c>
       <c r="AK18" t="s">
         <v>54</v>
@@ -3086,7 +3065,7 @@
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>9277</v>
+        <v>8079</v>
       </c>
       <c r="B19" t="s">
         <v>40</v>
@@ -3095,46 +3074,46 @@
         <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="F19">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="G19" t="s">
         <v>43</v>
       </c>
       <c r="H19" t="s">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="I19" t="s">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="J19">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
         <v>10</v>
       </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
       <c r="P19">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="Q19">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R19">
         <v>0</v>
@@ -3143,16 +3122,16 @@
         <v>0</v>
       </c>
       <c r="T19" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="U19" t="s">
-        <v>64</v>
+        <v>147</v>
       </c>
       <c r="V19" t="s">
         <v>48</v>
       </c>
       <c r="W19" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="X19">
         <v>0</v>
@@ -3161,13 +3140,13 @@
         <v>0</v>
       </c>
       <c r="Z19">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="AA19">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="AB19">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AC19">
         <v>0</v>
@@ -3179,19 +3158,19 @@
         <v>0</v>
       </c>
       <c r="AF19" t="s">
-        <v>47</v>
+        <v>166</v>
       </c>
       <c r="AG19">
         <v>1</v>
       </c>
       <c r="AH19" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="AI19">
         <v>0</v>
       </c>
       <c r="AJ19">
-        <v>36</v>
+        <v>251</v>
       </c>
       <c r="AK19" t="s">
         <v>54</v>
@@ -3202,7 +3181,7 @@
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>9922</v>
+        <v>10209</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
@@ -3211,25 +3190,25 @@
         <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="F20">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="G20" t="s">
         <v>43</v>
       </c>
       <c r="H20" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="I20" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="J20">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -3241,34 +3220,34 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O20">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P20">
         <v>20</v>
       </c>
       <c r="Q20">
+        <v>20</v>
+      </c>
+      <c r="R20">
         <v>10</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>20</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
       </c>
       <c r="T20" t="s">
         <v>63</v>
       </c>
       <c r="U20" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="V20" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="W20" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="X20">
         <v>0</v>
@@ -3277,25 +3256,25 @@
         <v>0</v>
       </c>
       <c r="Z20">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AA20">
+        <v>30</v>
+      </c>
+      <c r="AB20">
+        <v>30</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
         <v>20</v>
       </c>
-      <c r="AB20">
-        <v>60</v>
-      </c>
-      <c r="AC20">
-        <v>20</v>
-      </c>
-      <c r="AD20">
-        <v>0</v>
-      </c>
       <c r="AE20">
         <v>0</v>
       </c>
       <c r="AF20" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="AG20">
         <v>1</v>
@@ -3307,7 +3286,7 @@
         <v>0</v>
       </c>
       <c r="AJ20">
-        <v>16.25</v>
+        <v>44.33</v>
       </c>
       <c r="AK20" t="s">
         <v>54</v>
@@ -3318,34 +3297,34 @@
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>10074</v>
+        <v>3385</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>141</v>
+        <v>79</v>
       </c>
       <c r="E21" t="s">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="F21">
-        <v>156</v>
+        <v>65</v>
       </c>
       <c r="G21" t="s">
         <v>43</v>
       </c>
       <c r="H21" t="s">
-        <v>143</v>
+        <v>81</v>
       </c>
       <c r="I21" t="s">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="J21">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -3363,22 +3342,22 @@
         <v>0</v>
       </c>
       <c r="P21">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q21">
         <v>0</v>
       </c>
       <c r="R21">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="S21">
         <v>0</v>
       </c>
       <c r="T21" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="U21" t="s">
-        <v>145</v>
+        <v>84</v>
       </c>
       <c r="V21" t="s">
         <v>48</v>
@@ -3393,13 +3372,13 @@
         <v>0</v>
       </c>
       <c r="Z21">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="AA21">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AB21">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AC21">
         <v>0</v>
@@ -3411,7 +3390,7 @@
         <v>0</v>
       </c>
       <c r="AF21" t="s">
-        <v>145</v>
+        <v>84</v>
       </c>
       <c r="AG21">
         <v>1</v>
@@ -3423,7 +3402,7 @@
         <v>0</v>
       </c>
       <c r="AJ21">
-        <v>17.91</v>
+        <v>159</v>
       </c>
       <c r="AK21" t="s">
         <v>54</v>
@@ -3434,34 +3413,34 @@
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>10209</v>
+        <v>3171</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="F22">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="G22" t="s">
         <v>43</v>
       </c>
       <c r="H22" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="I22" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="J22">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -3473,34 +3452,34 @@
         <v>0</v>
       </c>
       <c r="N22">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
       <c r="P22">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q22">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="R22">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="S22">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T22" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="U22" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="V22" t="s">
         <v>65</v>
       </c>
       <c r="W22" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="X22">
         <v>0</v>
@@ -3509,75 +3488,75 @@
         <v>0</v>
       </c>
       <c r="Z22">
+        <v>40</v>
+      </c>
+      <c r="AA22">
+        <v>40</v>
+      </c>
+      <c r="AB22">
         <v>20</v>
       </c>
-      <c r="AA22">
-        <v>30</v>
-      </c>
-      <c r="AB22">
-        <v>30</v>
-      </c>
       <c r="AC22">
         <v>0</v>
       </c>
       <c r="AD22">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AE22">
         <v>0</v>
       </c>
       <c r="AF22" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="AG22">
         <v>1</v>
       </c>
       <c r="AH22" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="AI22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ22">
-        <v>44.33</v>
+        <v>85.86</v>
       </c>
       <c r="AK22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AL22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>10219</v>
+        <v>3880</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>149</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>151</v>
       </c>
       <c r="F23">
-        <v>160</v>
+        <v>42</v>
       </c>
       <c r="G23" t="s">
         <v>43</v>
       </c>
       <c r="H23" t="s">
-        <v>67</v>
+        <v>152</v>
       </c>
       <c r="I23" t="s">
-        <v>68</v>
+        <v>153</v>
       </c>
       <c r="J23">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -3586,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="M23">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -3595,22 +3574,22 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q23">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="R23">
         <v>20</v>
       </c>
       <c r="S23">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T23" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="U23" t="s">
-        <v>64</v>
+        <v>154</v>
       </c>
       <c r="V23" t="s">
         <v>48</v>
@@ -3622,16 +3601,16 @@
         <v>0</v>
       </c>
       <c r="Y23">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Z23">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="AA23">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="AB23">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AC23">
         <v>0</v>
@@ -3643,19 +3622,19 @@
         <v>0</v>
       </c>
       <c r="AF23" t="s">
-        <v>64</v>
+        <v>154</v>
       </c>
       <c r="AG23">
         <v>1</v>
       </c>
       <c r="AH23" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="AI23">
         <v>0</v>
       </c>
       <c r="AJ23">
-        <v>27.8</v>
+        <v>180</v>
       </c>
       <c r="AK23" t="s">
         <v>54</v>
@@ -3666,7 +3645,7 @@
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>10220</v>
+        <v>8230</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -3675,25 +3654,25 @@
         <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="F24">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="G24" t="s">
         <v>43</v>
       </c>
       <c r="H24" t="s">
-        <v>70</v>
+        <v>157</v>
       </c>
       <c r="I24" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="J24">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -3711,22 +3690,22 @@
         <v>0</v>
       </c>
       <c r="P24">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="Q24">
         <v>0</v>
       </c>
       <c r="R24">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="S24">
         <v>0</v>
       </c>
       <c r="T24" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="U24" t="s">
-        <v>64</v>
+        <v>147</v>
       </c>
       <c r="V24" t="s">
         <v>48</v>
@@ -3741,25 +3720,25 @@
         <v>0</v>
       </c>
       <c r="Z24">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="AA24">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="AB24">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="AC24">
         <v>0</v>
       </c>
       <c r="AD24">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AE24">
         <v>0</v>
       </c>
       <c r="AF24" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="AG24">
         <v>1</v>
@@ -3771,7 +3750,7 @@
         <v>0</v>
       </c>
       <c r="AJ24">
-        <v>34.85</v>
+        <v>41.69</v>
       </c>
       <c r="AK24" t="s">
         <v>54</v>
@@ -3782,43 +3761,43 @@
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>10446</v>
+        <v>1584</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="F25">
-        <v>159</v>
+        <v>85</v>
       </c>
       <c r="G25" t="s">
         <v>43</v>
       </c>
       <c r="H25" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="I25" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="J25">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M25">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -3839,34 +3818,34 @@
         <v>0</v>
       </c>
       <c r="T25" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="U25" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="V25" t="s">
         <v>48</v>
       </c>
       <c r="W25" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="X25">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="Y25">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Z25">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="AA25">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AB25">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AC25">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AD25">
         <v>0</v>
@@ -3875,30 +3854,30 @@
         <v>0</v>
       </c>
       <c r="AF25" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="AG25">
         <v>1</v>
       </c>
       <c r="AH25" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="AI25">
         <v>0</v>
       </c>
       <c r="AJ25">
-        <v>9.68</v>
+        <v>91.4</v>
       </c>
       <c r="AK25" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AL25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>10859</v>
+        <v>10219</v>
       </c>
       <c r="B26" t="s">
         <v>40</v>
@@ -3907,25 +3886,25 @@
         <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="F26">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G26" t="s">
         <v>43</v>
       </c>
       <c r="H26" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="I26" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="J26">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -3943,28 +3922,28 @@
         <v>0</v>
       </c>
       <c r="P26">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Q26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S26">
         <v>0</v>
       </c>
       <c r="T26" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="U26" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="V26" t="s">
         <v>48</v>
       </c>
       <c r="W26" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="X26">
         <v>0</v>
@@ -3973,14 +3952,14 @@
         <v>0</v>
       </c>
       <c r="Z26">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="AA26">
+        <v>40</v>
+      </c>
+      <c r="AB26">
         <v>20</v>
       </c>
-      <c r="AB26">
-        <v>0</v>
-      </c>
       <c r="AC26">
         <v>0</v>
       </c>
@@ -3991,7 +3970,7 @@
         <v>0</v>
       </c>
       <c r="AF26" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="AG26">
         <v>1</v>
@@ -4003,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="AJ26">
-        <v>10.8</v>
+        <v>27.8</v>
       </c>
       <c r="AK26" t="s">
         <v>54</v>
@@ -4014,34 +3993,34 @@
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>10860</v>
+        <v>3433</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="F27">
-        <v>161</v>
+        <v>65</v>
       </c>
       <c r="G27" t="s">
         <v>43</v>
       </c>
       <c r="H27" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="I27" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="J27">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -4065,22 +4044,22 @@
         <v>0</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="S27">
         <v>0</v>
       </c>
       <c r="T27" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="U27" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="V27" t="s">
         <v>48</v>
       </c>
       <c r="W27" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="X27">
         <v>0</v>
@@ -4089,16 +4068,16 @@
         <v>0</v>
       </c>
       <c r="Z27">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AA27">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="AB27">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="AC27">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="AD27">
         <v>0</v>
@@ -4107,7 +4086,7 @@
         <v>0</v>
       </c>
       <c r="AF27" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="AG27">
         <v>1</v>
@@ -4119,251 +4098,19 @@
         <v>0</v>
       </c>
       <c r="AJ27">
-        <v>8.1</v>
+        <v>56.6</v>
       </c>
       <c r="AK27" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AL27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>11221</v>
-      </c>
-      <c r="B28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E28" t="s">
-        <v>147</v>
-      </c>
-      <c r="F28">
-        <v>163</v>
-      </c>
-      <c r="G28" t="s">
-        <v>43</v>
-      </c>
-      <c r="H28" t="s">
-        <v>148</v>
-      </c>
-      <c r="I28" t="s">
-        <v>149</v>
-      </c>
-      <c r="J28">
-        <v>80</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28">
-        <v>20</v>
-      </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
-      <c r="S28">
-        <v>0</v>
-      </c>
-      <c r="T28" t="s">
-        <v>46</v>
-      </c>
-      <c r="U28" t="s">
-        <v>76</v>
-      </c>
-      <c r="V28" t="s">
-        <v>48</v>
-      </c>
-      <c r="W28" t="s">
-        <v>49</v>
-      </c>
-      <c r="X28">
-        <v>0</v>
-      </c>
-      <c r="Y28">
-        <v>0</v>
-      </c>
-      <c r="Z28">
-        <v>20</v>
-      </c>
-      <c r="AA28">
-        <v>50</v>
-      </c>
-      <c r="AB28">
-        <v>30</v>
-      </c>
-      <c r="AC28">
-        <v>0</v>
-      </c>
-      <c r="AD28">
-        <v>0</v>
-      </c>
-      <c r="AE28">
-        <v>0</v>
-      </c>
-      <c r="AF28" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG28">
-        <v>1</v>
-      </c>
-      <c r="AH28" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI28">
-        <v>0</v>
-      </c>
-      <c r="AJ28">
-        <v>11.83</v>
-      </c>
-      <c r="AK28" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>11778</v>
-      </c>
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" t="s">
-        <v>150</v>
-      </c>
-      <c r="E29" t="s">
-        <v>151</v>
-      </c>
-      <c r="F29">
-        <v>183</v>
-      </c>
-      <c r="G29" t="s">
-        <v>43</v>
-      </c>
-      <c r="H29" t="s">
-        <v>152</v>
-      </c>
-      <c r="I29" t="s">
-        <v>153</v>
-      </c>
-      <c r="J29">
-        <v>40</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <v>0</v>
-      </c>
-      <c r="P29">
-        <v>0</v>
-      </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <v>60</v>
-      </c>
-      <c r="S29">
-        <v>0</v>
-      </c>
-      <c r="T29" t="s">
-        <v>83</v>
-      </c>
-      <c r="U29" t="s">
-        <v>154</v>
-      </c>
-      <c r="V29" t="s">
-        <v>48</v>
-      </c>
-      <c r="W29" t="s">
-        <v>66</v>
-      </c>
-      <c r="X29">
-        <v>0</v>
-      </c>
-      <c r="Y29">
-        <v>0</v>
-      </c>
-      <c r="Z29">
-        <v>33</v>
-      </c>
-      <c r="AA29">
-        <v>33</v>
-      </c>
-      <c r="AB29">
-        <v>33</v>
-      </c>
-      <c r="AC29">
-        <v>0</v>
-      </c>
-      <c r="AD29">
-        <v>0</v>
-      </c>
-      <c r="AE29">
-        <v>0</v>
-      </c>
-      <c r="AF29" t="s">
-        <v>155</v>
-      </c>
-      <c r="AG29">
-        <v>1</v>
-      </c>
-      <c r="AH29" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI29">
-        <v>0</v>
-      </c>
-      <c r="AJ29">
-        <v>21.39</v>
-      </c>
-      <c r="AK29" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL29">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AN1" xr:uid="{584AC6E3-0767-6844-B41A-7765EF2908B7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AN29">
-      <sortCondition ref="A1:A29"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AN28">
+      <sortCondition ref="I1:I28"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>